<commit_message>
report9 get and show installmentFirstDate,LastDate
</commit_message>
<xml_diff>
--- a/jsreport-data/xlsx-template/report2489-template/contentRaw.xlsx
+++ b/jsreport-data/xlsx-template/report2489-template/contentRaw.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="42">
   <si>
     <t xml:space="preserve">ลำดับที่</t>
   </si>
@@ -577,10 +577,10 @@
     <t xml:space="preserve">วันที่ทำสัญญา</t>
   </si>
   <si>
-    <t xml:space="preserve">วันที่เริ่มสัญญา</t>
-  </si>
-  <si>
-    <t xml:space="preserve">วันที่สิ้นสุดสัญญา</t>
+    <t xml:space="preserve">วันที่ชำระงวดแรก</t>
+  </si>
+  <si>
+    <t xml:space="preserve">วันที่ชำระงวดสุดท้าย</t>
   </si>
   <si>
     <t xml:space="preserve">จำนวนงวดที่ต้องชำระ</t>
@@ -628,6 +628,9 @@
     </r>
   </si>
   <si>
+    <t xml:space="preserve">จำนวนเงินที่ต้องชำระ</t>
+  </si>
+  <si>
     <t xml:space="preserve">OFFICE</t>
   </si>
   <si>
@@ -646,6 +649,7 @@
         <color rgb="FF000000"/>
         <rFont val="DejaVu Sans"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">รวมช่องทาง </t>
     </r>
@@ -667,6 +671,7 @@
         <color rgb="FF000000"/>
         <rFont val="DejaVu Sans"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">รวมช่องทาง </t>
     </r>
@@ -688,6 +693,7 @@
         <color rgb="FF000000"/>
         <rFont val="DejaVu Sans"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">รวมช่องทาง </t>
     </r>
@@ -713,7 +719,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -750,12 +756,6 @@
       <name val="DejaVu Sans"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="DejaVu Sans"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="12">
@@ -874,7 +874,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="16">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -931,19 +931,11 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="8" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="9" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="9" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="10" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="10" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1026,8 +1018,8 @@
   </sheetPr>
   <dimension ref="A1:CG6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H4" activeCellId="0" sqref="H4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="BV1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="BZ7" activeCellId="0" sqref="BZ7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1035,13 +1027,13 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="9.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="9.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="9.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="9.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="7" style="0" width="10.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="10.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="10.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="11.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="13" style="0" width="10.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="13" style="0" width="10.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="11.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="11.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="18" style="0" width="11.14"/>
@@ -1559,13 +1551,13 @@
         <v>31</v>
       </c>
       <c r="CE5" s="12" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="CF5" s="12" t="s">
         <v>31</v>
       </c>
       <c r="CG5" s="12" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="56.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1579,196 +1571,196 @@
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
       <c r="J6" s="13" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="K6" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="L6" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="M6" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="N6" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="O6" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="L6" s="13" t="s">
+      <c r="P6" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="M6" s="14" t="s">
+      <c r="Q6" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="N6" s="14" t="s">
+      <c r="R6" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="S6" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="O6" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="P6" s="15" t="s">
+      <c r="T6" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="Q6" s="15" t="s">
+      <c r="U6" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="R6" s="16" t="s">
+      <c r="V6" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="S6" s="16" t="s">
+      <c r="W6" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="X6" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="T6" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="U6" s="13" t="s">
+      <c r="Y6" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="V6" s="13" t="s">
+      <c r="Z6" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="W6" s="14" t="s">
+      <c r="AA6" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="X6" s="14" t="s">
+      <c r="AB6" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="AC6" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="Y6" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="Z6" s="15" t="s">
+      <c r="AD6" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="AA6" s="15" t="s">
+      <c r="AE6" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="AB6" s="16" t="s">
+      <c r="AF6" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="AC6" s="16" t="s">
+      <c r="AG6" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="AH6" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="AD6" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="AE6" s="13" t="s">
+      <c r="AI6" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="AF6" s="13" t="s">
+      <c r="AJ6" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="AG6" s="14" t="s">
+      <c r="AK6" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="AH6" s="14" t="s">
+      <c r="AL6" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="AM6" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="AI6" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="AJ6" s="15" t="s">
+      <c r="AN6" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="AK6" s="15" t="s">
+      <c r="AO6" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="AL6" s="16" t="s">
+      <c r="AP6" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="AM6" s="16" t="s">
+      <c r="AQ6" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="AR6" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="AN6" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="AO6" s="13" t="s">
+      <c r="AS6" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="AP6" s="13" t="s">
+      <c r="AT6" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="AQ6" s="14" t="s">
+      <c r="AU6" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="AR6" s="14" t="s">
+      <c r="AV6" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="AW6" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="AS6" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="AT6" s="15" t="s">
+      <c r="AX6" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="AU6" s="15" t="s">
+      <c r="AY6" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="AV6" s="16" t="s">
+      <c r="AZ6" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="AW6" s="16" t="s">
+      <c r="BA6" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="BB6" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="AX6" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="AY6" s="13" t="s">
+      <c r="BC6" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="AZ6" s="13" t="s">
+      <c r="BD6" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="BA6" s="14" t="s">
+      <c r="BE6" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="BB6" s="14" t="s">
+      <c r="BF6" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="BG6" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="BC6" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="BD6" s="15" t="s">
+      <c r="BH6" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="BE6" s="15" t="s">
+      <c r="BI6" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="BF6" s="16" t="s">
+      <c r="BJ6" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="BG6" s="16" t="s">
+      <c r="BK6" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="BL6" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="BH6" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="BI6" s="13" t="s">
+      <c r="BM6" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="BJ6" s="13" t="s">
+      <c r="BN6" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="BK6" s="14" t="s">
+      <c r="BO6" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="BL6" s="14" t="s">
+      <c r="BP6" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="BQ6" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="BM6" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="BN6" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="BO6" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="BP6" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="BQ6" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="BR6" s="17" t="s">
-        <v>37</v>
-      </c>
-      <c r="BS6" s="17" t="s">
+      <c r="BR6" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="BT6" s="17" t="s">
+      <c r="BS6" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="BU6" s="17" t="s">
+      <c r="BT6" s="15" t="s">
         <v>40</v>
+      </c>
+      <c r="BU6" s="15" t="s">
+        <v>41</v>
       </c>
       <c r="BV6" s="11"/>
       <c r="BW6" s="4"/>

</xml_diff>